<commit_message>
Update ES2N-Requisitos Funcionais v3.0.xlsx
Atualização da descrição de RF07
</commit_message>
<xml_diff>
--- a/ES2N-Requisitos Funcionais v3.0.xlsx
+++ b/ES2N-Requisitos Funcionais v3.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus rubio\Documents\GitHub\TATUDOBEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULDADE\ES2\TATUDOBEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFABE7EC-CB63-484A-B2E3-35579C3AF09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64B8D34-9160-453D-A199-677BA1024DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
+    <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -147,9 +147,6 @@
     <t>O usuário administrador poderá cadastrar ou excluir categoria de receitas. (ex: salgado, doce)</t>
   </si>
   <si>
-    <t xml:space="preserve">O usuário administrador poderá cadastrar ou excluir subcategoria de receitas. (ex: salgado: torta, assados. doce: </t>
-  </si>
-  <si>
     <t>O usuário poderá pesquisar receitas no sistema. Essa busca pode ser feita de forma exclusiva (exatamente os ingredientes solicitados), ou abrangente (que contenham os ingredientes e mais outros).</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>DATA: 29/09/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O usuário administrador poderá cadastrar ou excluir subcategoria de receitas. (ex: salgado: torta, assados. doce: bolo, torta) </t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +634,7 @@
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -672,7 +672,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
@@ -782,7 +782,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>17</v>
@@ -818,13 +818,13 @@
         <v>20</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -907,7 +907,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>31</v>
@@ -925,18 +925,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1072,18 +1072,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9386896A-91B6-4EC7-AC94-350129FCA8CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9386896A-91B6-4EC7-AC94-350129FCA8CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>